<commit_message>
#72445 - Adicionar novas proveniencias
</commit_message>
<xml_diff>
--- a/excel/FolhaCod_ICD10_Int.xlsx
+++ b/excel/FolhaCod_ICD10_Int.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="19440" windowHeight="8445" tabRatio="644"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" tabRatio="644"/>
   </bookViews>
   <sheets>
     <sheet name="Int_Formato2" sheetId="12" r:id="rId1"/>
@@ -20,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="123">
   <si>
     <t>Hospital de Dia</t>
   </si>
@@ -392,6 +397,15 @@
   </si>
   <si>
     <t>Produção programada adicional</t>
+  </si>
+  <si>
+    <t>MCDT</t>
+  </si>
+  <si>
+    <t>Internamento</t>
+  </si>
+  <si>
+    <t>Outros</t>
   </si>
 </sst>
 </file>
@@ -544,7 +558,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -843,6 +857,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -850,7 +886,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="165">
+  <cellXfs count="167">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1095,6 +1131,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1167,7 +1204,8 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Euro" xfId="1"/>
@@ -1663,8 +1701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CF145"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="P118" sqref="P118"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="Q31" sqref="Q31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1815,33 +1853,33 @@
       <c r="AO2" s="93"/>
       <c r="AP2" s="93"/>
       <c r="AQ2" s="93"/>
-      <c r="AR2" s="140" t="s">
+      <c r="AR2" s="141" t="s">
         <v>51</v>
       </c>
-      <c r="AS2" s="141"/>
-      <c r="AT2" s="141"/>
-      <c r="AU2" s="141"/>
-      <c r="AV2" s="141"/>
-      <c r="AW2" s="141"/>
-      <c r="AX2" s="141"/>
-      <c r="AY2" s="141"/>
-      <c r="AZ2" s="141"/>
-      <c r="BA2" s="141"/>
-      <c r="BB2" s="141"/>
-      <c r="BC2" s="141"/>
-      <c r="BD2" s="141"/>
-      <c r="BE2" s="141"/>
-      <c r="BF2" s="141"/>
-      <c r="BG2" s="141"/>
-      <c r="BH2" s="141"/>
-      <c r="BI2" s="141"/>
-      <c r="BJ2" s="141"/>
-      <c r="BK2" s="141"/>
-      <c r="BL2" s="141"/>
-      <c r="BM2" s="141"/>
-      <c r="BN2" s="141"/>
-      <c r="BO2" s="141"/>
-      <c r="BP2" s="142"/>
+      <c r="AS2" s="142"/>
+      <c r="AT2" s="142"/>
+      <c r="AU2" s="142"/>
+      <c r="AV2" s="142"/>
+      <c r="AW2" s="142"/>
+      <c r="AX2" s="142"/>
+      <c r="AY2" s="142"/>
+      <c r="AZ2" s="142"/>
+      <c r="BA2" s="142"/>
+      <c r="BB2" s="142"/>
+      <c r="BC2" s="142"/>
+      <c r="BD2" s="142"/>
+      <c r="BE2" s="142"/>
+      <c r="BF2" s="142"/>
+      <c r="BG2" s="142"/>
+      <c r="BH2" s="142"/>
+      <c r="BI2" s="142"/>
+      <c r="BJ2" s="142"/>
+      <c r="BK2" s="142"/>
+      <c r="BL2" s="142"/>
+      <c r="BM2" s="142"/>
+      <c r="BN2" s="142"/>
+      <c r="BO2" s="142"/>
+      <c r="BP2" s="143"/>
     </row>
     <row r="3" spans="2:69" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="91"/>
@@ -1886,31 +1924,31 @@
       <c r="AO3" s="93"/>
       <c r="AP3" s="93"/>
       <c r="AQ3" s="93"/>
-      <c r="AR3" s="143"/>
-      <c r="AS3" s="144"/>
-      <c r="AT3" s="144"/>
-      <c r="AU3" s="144"/>
-      <c r="AV3" s="144"/>
-      <c r="AW3" s="144"/>
-      <c r="AX3" s="144"/>
-      <c r="AY3" s="144"/>
-      <c r="AZ3" s="144"/>
-      <c r="BA3" s="144"/>
-      <c r="BB3" s="144"/>
-      <c r="BC3" s="144"/>
-      <c r="BD3" s="144"/>
-      <c r="BE3" s="144"/>
-      <c r="BF3" s="144"/>
-      <c r="BG3" s="144"/>
-      <c r="BH3" s="144"/>
-      <c r="BI3" s="144"/>
-      <c r="BJ3" s="144"/>
-      <c r="BK3" s="144"/>
-      <c r="BL3" s="144"/>
-      <c r="BM3" s="144"/>
-      <c r="BN3" s="144"/>
-      <c r="BO3" s="144"/>
-      <c r="BP3" s="145"/>
+      <c r="AR3" s="144"/>
+      <c r="AS3" s="145"/>
+      <c r="AT3" s="145"/>
+      <c r="AU3" s="145"/>
+      <c r="AV3" s="145"/>
+      <c r="AW3" s="145"/>
+      <c r="AX3" s="145"/>
+      <c r="AY3" s="145"/>
+      <c r="AZ3" s="145"/>
+      <c r="BA3" s="145"/>
+      <c r="BB3" s="145"/>
+      <c r="BC3" s="145"/>
+      <c r="BD3" s="145"/>
+      <c r="BE3" s="145"/>
+      <c r="BF3" s="145"/>
+      <c r="BG3" s="145"/>
+      <c r="BH3" s="145"/>
+      <c r="BI3" s="145"/>
+      <c r="BJ3" s="145"/>
+      <c r="BK3" s="145"/>
+      <c r="BL3" s="145"/>
+      <c r="BM3" s="145"/>
+      <c r="BN3" s="145"/>
+      <c r="BO3" s="145"/>
+      <c r="BP3" s="146"/>
     </row>
     <row r="4" spans="2:69" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="96"/>
@@ -1955,31 +1993,31 @@
       <c r="AO4" s="101"/>
       <c r="AP4" s="101"/>
       <c r="AQ4" s="93"/>
-      <c r="AR4" s="146"/>
-      <c r="AS4" s="147"/>
-      <c r="AT4" s="147"/>
-      <c r="AU4" s="147"/>
-      <c r="AV4" s="147"/>
-      <c r="AW4" s="147"/>
-      <c r="AX4" s="147"/>
-      <c r="AY4" s="147"/>
-      <c r="AZ4" s="147"/>
-      <c r="BA4" s="147"/>
-      <c r="BB4" s="147"/>
-      <c r="BC4" s="147"/>
-      <c r="BD4" s="147"/>
-      <c r="BE4" s="147"/>
-      <c r="BF4" s="147"/>
-      <c r="BG4" s="147"/>
-      <c r="BH4" s="147"/>
-      <c r="BI4" s="147"/>
-      <c r="BJ4" s="147"/>
-      <c r="BK4" s="147"/>
-      <c r="BL4" s="147"/>
-      <c r="BM4" s="147"/>
-      <c r="BN4" s="147"/>
-      <c r="BO4" s="147"/>
-      <c r="BP4" s="148"/>
+      <c r="AR4" s="147"/>
+      <c r="AS4" s="148"/>
+      <c r="AT4" s="148"/>
+      <c r="AU4" s="148"/>
+      <c r="AV4" s="148"/>
+      <c r="AW4" s="148"/>
+      <c r="AX4" s="148"/>
+      <c r="AY4" s="148"/>
+      <c r="AZ4" s="148"/>
+      <c r="BA4" s="148"/>
+      <c r="BB4" s="148"/>
+      <c r="BC4" s="148"/>
+      <c r="BD4" s="148"/>
+      <c r="BE4" s="148"/>
+      <c r="BF4" s="148"/>
+      <c r="BG4" s="148"/>
+      <c r="BH4" s="148"/>
+      <c r="BI4" s="148"/>
+      <c r="BJ4" s="148"/>
+      <c r="BK4" s="148"/>
+      <c r="BL4" s="148"/>
+      <c r="BM4" s="148"/>
+      <c r="BN4" s="148"/>
+      <c r="BO4" s="148"/>
+      <c r="BP4" s="149"/>
     </row>
     <row r="5" spans="2:69" ht="4.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="96"/>
@@ -2051,75 +2089,75 @@
       <c r="BP5" s="123"/>
     </row>
     <row r="6" spans="2:69" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="149" t="s">
+      <c r="B6" s="150" t="s">
         <v>83</v>
       </c>
-      <c r="C6" s="150"/>
-      <c r="D6" s="150"/>
-      <c r="E6" s="150"/>
-      <c r="F6" s="150"/>
-      <c r="G6" s="150"/>
-      <c r="H6" s="150"/>
-      <c r="I6" s="150"/>
-      <c r="J6" s="150"/>
-      <c r="K6" s="150"/>
-      <c r="L6" s="151"/>
-      <c r="M6" s="151"/>
-      <c r="N6" s="151"/>
-      <c r="O6" s="151"/>
-      <c r="P6" s="151"/>
-      <c r="Q6" s="151"/>
-      <c r="R6" s="151"/>
-      <c r="S6" s="151"/>
-      <c r="T6" s="151"/>
-      <c r="U6" s="151"/>
-      <c r="V6" s="151"/>
-      <c r="W6" s="151"/>
-      <c r="X6" s="151"/>
-      <c r="Y6" s="151"/>
-      <c r="Z6" s="151"/>
-      <c r="AA6" s="151"/>
-      <c r="AB6" s="151"/>
-      <c r="AC6" s="151"/>
-      <c r="AD6" s="151"/>
-      <c r="AE6" s="151"/>
-      <c r="AF6" s="151"/>
-      <c r="AG6" s="151"/>
-      <c r="AH6" s="151"/>
-      <c r="AI6" s="151"/>
-      <c r="AJ6" s="151"/>
-      <c r="AK6" s="151"/>
-      <c r="AL6" s="151"/>
-      <c r="AM6" s="151"/>
-      <c r="AN6" s="151"/>
-      <c r="AO6" s="151"/>
-      <c r="AP6" s="151"/>
-      <c r="AQ6" s="151"/>
-      <c r="AR6" s="151"/>
-      <c r="AS6" s="151"/>
-      <c r="AT6" s="151"/>
-      <c r="AU6" s="151"/>
-      <c r="AV6" s="151"/>
-      <c r="AW6" s="151"/>
-      <c r="AX6" s="151"/>
-      <c r="AY6" s="151"/>
-      <c r="AZ6" s="151"/>
-      <c r="BA6" s="151"/>
-      <c r="BB6" s="151"/>
-      <c r="BC6" s="151"/>
-      <c r="BD6" s="151"/>
-      <c r="BE6" s="151"/>
-      <c r="BF6" s="151"/>
-      <c r="BG6" s="151"/>
-      <c r="BH6" s="151"/>
-      <c r="BI6" s="151"/>
-      <c r="BJ6" s="151"/>
-      <c r="BK6" s="151"/>
-      <c r="BL6" s="151"/>
-      <c r="BM6" s="151"/>
-      <c r="BN6" s="151"/>
-      <c r="BO6" s="151"/>
-      <c r="BP6" s="152"/>
+      <c r="C6" s="151"/>
+      <c r="D6" s="151"/>
+      <c r="E6" s="151"/>
+      <c r="F6" s="151"/>
+      <c r="G6" s="151"/>
+      <c r="H6" s="151"/>
+      <c r="I6" s="151"/>
+      <c r="J6" s="151"/>
+      <c r="K6" s="151"/>
+      <c r="L6" s="152"/>
+      <c r="M6" s="152"/>
+      <c r="N6" s="152"/>
+      <c r="O6" s="152"/>
+      <c r="P6" s="152"/>
+      <c r="Q6" s="152"/>
+      <c r="R6" s="152"/>
+      <c r="S6" s="152"/>
+      <c r="T6" s="152"/>
+      <c r="U6" s="152"/>
+      <c r="V6" s="152"/>
+      <c r="W6" s="152"/>
+      <c r="X6" s="152"/>
+      <c r="Y6" s="152"/>
+      <c r="Z6" s="152"/>
+      <c r="AA6" s="152"/>
+      <c r="AB6" s="152"/>
+      <c r="AC6" s="152"/>
+      <c r="AD6" s="152"/>
+      <c r="AE6" s="152"/>
+      <c r="AF6" s="152"/>
+      <c r="AG6" s="152"/>
+      <c r="AH6" s="152"/>
+      <c r="AI6" s="152"/>
+      <c r="AJ6" s="152"/>
+      <c r="AK6" s="152"/>
+      <c r="AL6" s="152"/>
+      <c r="AM6" s="152"/>
+      <c r="AN6" s="152"/>
+      <c r="AO6" s="152"/>
+      <c r="AP6" s="152"/>
+      <c r="AQ6" s="152"/>
+      <c r="AR6" s="152"/>
+      <c r="AS6" s="152"/>
+      <c r="AT6" s="152"/>
+      <c r="AU6" s="152"/>
+      <c r="AV6" s="152"/>
+      <c r="AW6" s="152"/>
+      <c r="AX6" s="152"/>
+      <c r="AY6" s="152"/>
+      <c r="AZ6" s="152"/>
+      <c r="BA6" s="152"/>
+      <c r="BB6" s="152"/>
+      <c r="BC6" s="152"/>
+      <c r="BD6" s="152"/>
+      <c r="BE6" s="152"/>
+      <c r="BF6" s="152"/>
+      <c r="BG6" s="152"/>
+      <c r="BH6" s="152"/>
+      <c r="BI6" s="152"/>
+      <c r="BJ6" s="152"/>
+      <c r="BK6" s="152"/>
+      <c r="BL6" s="152"/>
+      <c r="BM6" s="152"/>
+      <c r="BN6" s="152"/>
+      <c r="BO6" s="152"/>
+      <c r="BP6" s="153"/>
     </row>
     <row r="7" spans="2:69" s="17" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="13"/>
@@ -2771,75 +2809,75 @@
       <c r="BQ15" s="5"/>
     </row>
     <row r="16" spans="2:69" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="156" t="s">
+      <c r="B16" s="157" t="s">
         <v>59</v>
       </c>
-      <c r="C16" s="151"/>
-      <c r="D16" s="151"/>
-      <c r="E16" s="151"/>
-      <c r="F16" s="151"/>
-      <c r="G16" s="151"/>
-      <c r="H16" s="151"/>
-      <c r="I16" s="151"/>
-      <c r="J16" s="151"/>
-      <c r="K16" s="151"/>
-      <c r="L16" s="151"/>
-      <c r="M16" s="151"/>
-      <c r="N16" s="151"/>
-      <c r="O16" s="151"/>
-      <c r="P16" s="151"/>
-      <c r="Q16" s="151"/>
-      <c r="R16" s="151"/>
-      <c r="S16" s="151"/>
-      <c r="T16" s="151"/>
-      <c r="U16" s="151"/>
-      <c r="V16" s="151"/>
-      <c r="W16" s="151"/>
-      <c r="X16" s="151"/>
-      <c r="Y16" s="151"/>
-      <c r="Z16" s="151"/>
-      <c r="AA16" s="151"/>
-      <c r="AB16" s="151"/>
-      <c r="AC16" s="151"/>
-      <c r="AD16" s="151"/>
-      <c r="AE16" s="151"/>
-      <c r="AF16" s="151"/>
-      <c r="AG16" s="151"/>
-      <c r="AH16" s="151"/>
-      <c r="AI16" s="151"/>
-      <c r="AJ16" s="151"/>
-      <c r="AK16" s="151"/>
-      <c r="AL16" s="151"/>
-      <c r="AM16" s="151"/>
-      <c r="AN16" s="151"/>
-      <c r="AO16" s="151"/>
-      <c r="AP16" s="151"/>
-      <c r="AQ16" s="151"/>
-      <c r="AR16" s="151"/>
-      <c r="AS16" s="151"/>
-      <c r="AT16" s="151"/>
-      <c r="AU16" s="151"/>
-      <c r="AV16" s="151"/>
-      <c r="AW16" s="151"/>
-      <c r="AX16" s="151"/>
-      <c r="AY16" s="151"/>
-      <c r="AZ16" s="151"/>
-      <c r="BA16" s="151"/>
-      <c r="BB16" s="151"/>
-      <c r="BC16" s="151"/>
-      <c r="BD16" s="151"/>
-      <c r="BE16" s="151"/>
-      <c r="BF16" s="151"/>
-      <c r="BG16" s="151"/>
-      <c r="BH16" s="151"/>
-      <c r="BI16" s="151"/>
-      <c r="BJ16" s="151"/>
-      <c r="BK16" s="151"/>
-      <c r="BL16" s="151"/>
-      <c r="BM16" s="151"/>
-      <c r="BN16" s="151"/>
-      <c r="BO16" s="151"/>
-      <c r="BP16" s="152"/>
+      <c r="C16" s="152"/>
+      <c r="D16" s="152"/>
+      <c r="E16" s="152"/>
+      <c r="F16" s="152"/>
+      <c r="G16" s="152"/>
+      <c r="H16" s="152"/>
+      <c r="I16" s="152"/>
+      <c r="J16" s="152"/>
+      <c r="K16" s="152"/>
+      <c r="L16" s="152"/>
+      <c r="M16" s="152"/>
+      <c r="N16" s="152"/>
+      <c r="O16" s="152"/>
+      <c r="P16" s="152"/>
+      <c r="Q16" s="152"/>
+      <c r="R16" s="152"/>
+      <c r="S16" s="152"/>
+      <c r="T16" s="152"/>
+      <c r="U16" s="152"/>
+      <c r="V16" s="152"/>
+      <c r="W16" s="152"/>
+      <c r="X16" s="152"/>
+      <c r="Y16" s="152"/>
+      <c r="Z16" s="152"/>
+      <c r="AA16" s="152"/>
+      <c r="AB16" s="152"/>
+      <c r="AC16" s="152"/>
+      <c r="AD16" s="152"/>
+      <c r="AE16" s="152"/>
+      <c r="AF16" s="152"/>
+      <c r="AG16" s="152"/>
+      <c r="AH16" s="152"/>
+      <c r="AI16" s="152"/>
+      <c r="AJ16" s="152"/>
+      <c r="AK16" s="152"/>
+      <c r="AL16" s="152"/>
+      <c r="AM16" s="152"/>
+      <c r="AN16" s="152"/>
+      <c r="AO16" s="152"/>
+      <c r="AP16" s="152"/>
+      <c r="AQ16" s="152"/>
+      <c r="AR16" s="152"/>
+      <c r="AS16" s="152"/>
+      <c r="AT16" s="152"/>
+      <c r="AU16" s="152"/>
+      <c r="AV16" s="152"/>
+      <c r="AW16" s="152"/>
+      <c r="AX16" s="152"/>
+      <c r="AY16" s="152"/>
+      <c r="AZ16" s="152"/>
+      <c r="BA16" s="152"/>
+      <c r="BB16" s="152"/>
+      <c r="BC16" s="152"/>
+      <c r="BD16" s="152"/>
+      <c r="BE16" s="152"/>
+      <c r="BF16" s="152"/>
+      <c r="BG16" s="152"/>
+      <c r="BH16" s="152"/>
+      <c r="BI16" s="152"/>
+      <c r="BJ16" s="152"/>
+      <c r="BK16" s="152"/>
+      <c r="BL16" s="152"/>
+      <c r="BM16" s="152"/>
+      <c r="BN16" s="152"/>
+      <c r="BO16" s="152"/>
+      <c r="BP16" s="153"/>
       <c r="BQ16" s="5"/>
     </row>
     <row r="17" spans="2:69" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3200,77 +3238,77 @@
       <c r="BQ21" s="5"/>
     </row>
     <row r="22" spans="2:69" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="156" t="s">
+      <c r="B22" s="157" t="s">
         <v>42</v>
       </c>
-      <c r="C22" s="151"/>
-      <c r="D22" s="151"/>
-      <c r="E22" s="151"/>
-      <c r="F22" s="151"/>
-      <c r="G22" s="151"/>
-      <c r="H22" s="151"/>
-      <c r="I22" s="151"/>
-      <c r="J22" s="151"/>
-      <c r="K22" s="151"/>
-      <c r="L22" s="151"/>
-      <c r="M22" s="151"/>
-      <c r="N22" s="151"/>
-      <c r="O22" s="151"/>
-      <c r="P22" s="151"/>
-      <c r="Q22" s="151"/>
-      <c r="R22" s="151"/>
-      <c r="S22" s="151"/>
-      <c r="T22" s="151"/>
-      <c r="U22" s="151"/>
-      <c r="V22" s="152"/>
-      <c r="W22" s="153" t="s">
+      <c r="C22" s="152"/>
+      <c r="D22" s="152"/>
+      <c r="E22" s="152"/>
+      <c r="F22" s="152"/>
+      <c r="G22" s="152"/>
+      <c r="H22" s="152"/>
+      <c r="I22" s="152"/>
+      <c r="J22" s="152"/>
+      <c r="K22" s="152"/>
+      <c r="L22" s="152"/>
+      <c r="M22" s="152"/>
+      <c r="N22" s="152"/>
+      <c r="O22" s="152"/>
+      <c r="P22" s="152"/>
+      <c r="Q22" s="152"/>
+      <c r="R22" s="152"/>
+      <c r="S22" s="152"/>
+      <c r="T22" s="152"/>
+      <c r="U22" s="152"/>
+      <c r="V22" s="153"/>
+      <c r="W22" s="154" t="s">
         <v>28</v>
       </c>
-      <c r="X22" s="154"/>
-      <c r="Y22" s="154"/>
-      <c r="Z22" s="154"/>
-      <c r="AA22" s="154"/>
-      <c r="AB22" s="154"/>
-      <c r="AC22" s="154"/>
-      <c r="AD22" s="154"/>
-      <c r="AE22" s="154"/>
-      <c r="AF22" s="154"/>
-      <c r="AG22" s="154"/>
-      <c r="AH22" s="154"/>
-      <c r="AI22" s="154"/>
-      <c r="AJ22" s="154"/>
-      <c r="AK22" s="154"/>
-      <c r="AL22" s="154"/>
-      <c r="AM22" s="154"/>
-      <c r="AN22" s="154"/>
-      <c r="AO22" s="154"/>
-      <c r="AP22" s="154"/>
-      <c r="AQ22" s="154"/>
-      <c r="AR22" s="154"/>
-      <c r="AS22" s="154"/>
-      <c r="AT22" s="154"/>
-      <c r="AU22" s="154"/>
-      <c r="AV22" s="154"/>
-      <c r="AW22" s="154"/>
-      <c r="AX22" s="154"/>
-      <c r="AY22" s="154"/>
-      <c r="AZ22" s="154"/>
-      <c r="BA22" s="154"/>
-      <c r="BB22" s="154"/>
-      <c r="BC22" s="154"/>
-      <c r="BD22" s="154"/>
-      <c r="BE22" s="154"/>
-      <c r="BF22" s="154"/>
-      <c r="BG22" s="154"/>
-      <c r="BH22" s="154"/>
-      <c r="BI22" s="154"/>
-      <c r="BJ22" s="154"/>
-      <c r="BK22" s="154"/>
-      <c r="BL22" s="154"/>
-      <c r="BM22" s="154"/>
-      <c r="BN22" s="154"/>
-      <c r="BO22" s="154"/>
-      <c r="BP22" s="155"/>
+      <c r="X22" s="155"/>
+      <c r="Y22" s="155"/>
+      <c r="Z22" s="155"/>
+      <c r="AA22" s="155"/>
+      <c r="AB22" s="155"/>
+      <c r="AC22" s="155"/>
+      <c r="AD22" s="155"/>
+      <c r="AE22" s="155"/>
+      <c r="AF22" s="155"/>
+      <c r="AG22" s="155"/>
+      <c r="AH22" s="155"/>
+      <c r="AI22" s="155"/>
+      <c r="AJ22" s="155"/>
+      <c r="AK22" s="155"/>
+      <c r="AL22" s="155"/>
+      <c r="AM22" s="155"/>
+      <c r="AN22" s="155"/>
+      <c r="AO22" s="155"/>
+      <c r="AP22" s="155"/>
+      <c r="AQ22" s="155"/>
+      <c r="AR22" s="155"/>
+      <c r="AS22" s="155"/>
+      <c r="AT22" s="155"/>
+      <c r="AU22" s="155"/>
+      <c r="AV22" s="155"/>
+      <c r="AW22" s="155"/>
+      <c r="AX22" s="155"/>
+      <c r="AY22" s="155"/>
+      <c r="AZ22" s="155"/>
+      <c r="BA22" s="155"/>
+      <c r="BB22" s="155"/>
+      <c r="BC22" s="155"/>
+      <c r="BD22" s="155"/>
+      <c r="BE22" s="155"/>
+      <c r="BF22" s="155"/>
+      <c r="BG22" s="155"/>
+      <c r="BH22" s="155"/>
+      <c r="BI22" s="155"/>
+      <c r="BJ22" s="155"/>
+      <c r="BK22" s="155"/>
+      <c r="BL22" s="155"/>
+      <c r="BM22" s="155"/>
+      <c r="BN22" s="155"/>
+      <c r="BO22" s="155"/>
+      <c r="BP22" s="156"/>
       <c r="BQ22" s="5"/>
     </row>
     <row r="23" spans="2:69" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3535,9 +3573,11 @@
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
-      <c r="M28" s="5"/>
+      <c r="M28" s="127"/>
       <c r="N28" s="112"/>
-      <c r="O28" s="112"/>
+      <c r="O28" s="5" t="s">
+        <v>120</v>
+      </c>
       <c r="P28" s="112"/>
       <c r="Q28" s="112"/>
       <c r="R28" s="112"/>
@@ -3610,9 +3650,11 @@
       <c r="J29" s="37"/>
       <c r="K29" s="37"/>
       <c r="L29" s="5"/>
-      <c r="M29" s="5"/>
+      <c r="M29" s="127"/>
       <c r="N29" s="112"/>
-      <c r="O29" s="112"/>
+      <c r="O29" s="5" t="s">
+        <v>121</v>
+      </c>
       <c r="P29" s="112"/>
       <c r="Q29" s="125"/>
       <c r="R29" s="125"/>
@@ -3681,14 +3723,16 @@
       <c r="J30" s="37"/>
       <c r="K30" s="37"/>
       <c r="L30" s="5"/>
-      <c r="M30" s="5"/>
+      <c r="M30" s="127"/>
       <c r="N30" s="112"/>
-      <c r="O30" s="112"/>
+      <c r="O30" s="5" t="s">
+        <v>122</v>
+      </c>
       <c r="P30" s="112"/>
       <c r="Q30" s="125"/>
       <c r="R30" s="125"/>
       <c r="S30" s="125"/>
-      <c r="T30" s="127"/>
+      <c r="T30" s="165"/>
       <c r="U30" s="125"/>
       <c r="V30" s="132"/>
       <c r="W30" s="4"/>
@@ -3756,14 +3800,14 @@
       <c r="J31" s="37"/>
       <c r="K31" s="37"/>
       <c r="L31" s="5"/>
-      <c r="M31" s="5"/>
+      <c r="M31" s="127"/>
       <c r="N31" s="112"/>
       <c r="O31" s="112"/>
       <c r="P31" s="112"/>
       <c r="Q31" s="125"/>
       <c r="R31" s="125"/>
       <c r="S31" s="125"/>
-      <c r="T31" s="127"/>
+      <c r="T31" s="166"/>
       <c r="U31" s="125"/>
       <c r="V31" s="132"/>
       <c r="W31" s="4"/>
@@ -4248,29 +4292,29 @@
       <c r="BQ37" s="5"/>
     </row>
     <row r="38" spans="1:69" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="156" t="s">
+      <c r="B38" s="157" t="s">
         <v>90</v>
       </c>
-      <c r="C38" s="151"/>
-      <c r="D38" s="151"/>
-      <c r="E38" s="151"/>
-      <c r="F38" s="151"/>
-      <c r="G38" s="151"/>
-      <c r="H38" s="151"/>
-      <c r="I38" s="151"/>
-      <c r="J38" s="151"/>
-      <c r="K38" s="151"/>
-      <c r="L38" s="151"/>
-      <c r="M38" s="151"/>
-      <c r="N38" s="151"/>
-      <c r="O38" s="151"/>
-      <c r="P38" s="151"/>
-      <c r="Q38" s="151"/>
-      <c r="R38" s="151"/>
-      <c r="S38" s="151"/>
-      <c r="T38" s="151"/>
-      <c r="U38" s="151"/>
-      <c r="V38" s="152"/>
+      <c r="C38" s="152"/>
+      <c r="D38" s="152"/>
+      <c r="E38" s="152"/>
+      <c r="F38" s="152"/>
+      <c r="G38" s="152"/>
+      <c r="H38" s="152"/>
+      <c r="I38" s="152"/>
+      <c r="J38" s="152"/>
+      <c r="K38" s="152"/>
+      <c r="L38" s="152"/>
+      <c r="M38" s="152"/>
+      <c r="N38" s="152"/>
+      <c r="O38" s="152"/>
+      <c r="P38" s="152"/>
+      <c r="Q38" s="152"/>
+      <c r="R38" s="152"/>
+      <c r="S38" s="152"/>
+      <c r="T38" s="152"/>
+      <c r="U38" s="152"/>
+      <c r="V38" s="153"/>
       <c r="W38" s="4"/>
       <c r="X38" s="48" t="s">
         <v>20</v>
@@ -4996,75 +5040,75 @@
       <c r="BQ49" s="5"/>
     </row>
     <row r="50" spans="1:84" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="157" t="s">
+      <c r="B50" s="158" t="s">
         <v>115</v>
       </c>
-      <c r="C50" s="158"/>
-      <c r="D50" s="158"/>
-      <c r="E50" s="158"/>
-      <c r="F50" s="158"/>
-      <c r="G50" s="158"/>
-      <c r="H50" s="158"/>
-      <c r="I50" s="158"/>
-      <c r="J50" s="158"/>
-      <c r="K50" s="158"/>
-      <c r="L50" s="158"/>
-      <c r="M50" s="158"/>
-      <c r="N50" s="158"/>
-      <c r="O50" s="158"/>
-      <c r="P50" s="158"/>
-      <c r="Q50" s="158"/>
-      <c r="R50" s="158"/>
-      <c r="S50" s="158"/>
-      <c r="T50" s="158"/>
-      <c r="U50" s="158"/>
-      <c r="V50" s="158"/>
-      <c r="W50" s="158"/>
-      <c r="X50" s="158"/>
-      <c r="Y50" s="158"/>
-      <c r="Z50" s="158"/>
-      <c r="AA50" s="158"/>
-      <c r="AB50" s="158"/>
-      <c r="AC50" s="158"/>
-      <c r="AD50" s="158"/>
-      <c r="AE50" s="158"/>
-      <c r="AF50" s="158"/>
-      <c r="AG50" s="158"/>
-      <c r="AH50" s="158"/>
-      <c r="AI50" s="158"/>
-      <c r="AJ50" s="158"/>
-      <c r="AK50" s="158"/>
-      <c r="AL50" s="158"/>
-      <c r="AM50" s="158"/>
-      <c r="AN50" s="158"/>
-      <c r="AO50" s="158"/>
-      <c r="AP50" s="158"/>
-      <c r="AQ50" s="158"/>
-      <c r="AR50" s="158"/>
-      <c r="AS50" s="158"/>
-      <c r="AT50" s="158"/>
-      <c r="AU50" s="158"/>
-      <c r="AV50" s="158"/>
-      <c r="AW50" s="158"/>
-      <c r="AX50" s="158"/>
-      <c r="AY50" s="158"/>
-      <c r="AZ50" s="158"/>
-      <c r="BA50" s="158"/>
-      <c r="BB50" s="158"/>
-      <c r="BC50" s="158"/>
-      <c r="BD50" s="158"/>
-      <c r="BE50" s="158"/>
-      <c r="BF50" s="158"/>
-      <c r="BG50" s="158"/>
-      <c r="BH50" s="158"/>
-      <c r="BI50" s="158"/>
-      <c r="BJ50" s="158"/>
-      <c r="BK50" s="158"/>
-      <c r="BL50" s="158"/>
-      <c r="BM50" s="158"/>
-      <c r="BN50" s="158"/>
-      <c r="BO50" s="158"/>
-      <c r="BP50" s="159"/>
+      <c r="C50" s="159"/>
+      <c r="D50" s="159"/>
+      <c r="E50" s="159"/>
+      <c r="F50" s="159"/>
+      <c r="G50" s="159"/>
+      <c r="H50" s="159"/>
+      <c r="I50" s="159"/>
+      <c r="J50" s="159"/>
+      <c r="K50" s="159"/>
+      <c r="L50" s="159"/>
+      <c r="M50" s="159"/>
+      <c r="N50" s="159"/>
+      <c r="O50" s="159"/>
+      <c r="P50" s="159"/>
+      <c r="Q50" s="159"/>
+      <c r="R50" s="159"/>
+      <c r="S50" s="159"/>
+      <c r="T50" s="159"/>
+      <c r="U50" s="159"/>
+      <c r="V50" s="159"/>
+      <c r="W50" s="159"/>
+      <c r="X50" s="159"/>
+      <c r="Y50" s="159"/>
+      <c r="Z50" s="159"/>
+      <c r="AA50" s="159"/>
+      <c r="AB50" s="159"/>
+      <c r="AC50" s="159"/>
+      <c r="AD50" s="159"/>
+      <c r="AE50" s="159"/>
+      <c r="AF50" s="159"/>
+      <c r="AG50" s="159"/>
+      <c r="AH50" s="159"/>
+      <c r="AI50" s="159"/>
+      <c r="AJ50" s="159"/>
+      <c r="AK50" s="159"/>
+      <c r="AL50" s="159"/>
+      <c r="AM50" s="159"/>
+      <c r="AN50" s="159"/>
+      <c r="AO50" s="159"/>
+      <c r="AP50" s="159"/>
+      <c r="AQ50" s="159"/>
+      <c r="AR50" s="159"/>
+      <c r="AS50" s="159"/>
+      <c r="AT50" s="159"/>
+      <c r="AU50" s="159"/>
+      <c r="AV50" s="159"/>
+      <c r="AW50" s="159"/>
+      <c r="AX50" s="159"/>
+      <c r="AY50" s="159"/>
+      <c r="AZ50" s="159"/>
+      <c r="BA50" s="159"/>
+      <c r="BB50" s="159"/>
+      <c r="BC50" s="159"/>
+      <c r="BD50" s="159"/>
+      <c r="BE50" s="159"/>
+      <c r="BF50" s="159"/>
+      <c r="BG50" s="159"/>
+      <c r="BH50" s="159"/>
+      <c r="BI50" s="159"/>
+      <c r="BJ50" s="159"/>
+      <c r="BK50" s="159"/>
+      <c r="BL50" s="159"/>
+      <c r="BM50" s="159"/>
+      <c r="BN50" s="159"/>
+      <c r="BO50" s="159"/>
+      <c r="BP50" s="160"/>
       <c r="BQ50" s="37"/>
       <c r="BR50" s="37"/>
       <c r="BS50" s="37"/>
@@ -5210,75 +5254,75 @@
       <c r="BU52" s="37"/>
     </row>
     <row r="53" spans="1:84" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="157" t="s">
+      <c r="B53" s="158" t="s">
         <v>117</v>
       </c>
-      <c r="C53" s="158"/>
-      <c r="D53" s="158"/>
-      <c r="E53" s="158"/>
-      <c r="F53" s="158"/>
-      <c r="G53" s="158"/>
-      <c r="H53" s="158"/>
-      <c r="I53" s="158"/>
-      <c r="J53" s="158"/>
-      <c r="K53" s="158"/>
-      <c r="L53" s="158"/>
-      <c r="M53" s="158"/>
-      <c r="N53" s="158"/>
-      <c r="O53" s="158"/>
-      <c r="P53" s="158"/>
-      <c r="Q53" s="158"/>
-      <c r="R53" s="158"/>
-      <c r="S53" s="158"/>
-      <c r="T53" s="158"/>
-      <c r="U53" s="158"/>
-      <c r="V53" s="158"/>
-      <c r="W53" s="158"/>
-      <c r="X53" s="158"/>
-      <c r="Y53" s="158"/>
-      <c r="Z53" s="158"/>
-      <c r="AA53" s="158"/>
-      <c r="AB53" s="158"/>
-      <c r="AC53" s="158"/>
-      <c r="AD53" s="158"/>
-      <c r="AE53" s="158"/>
-      <c r="AF53" s="158"/>
-      <c r="AG53" s="158"/>
-      <c r="AH53" s="158"/>
-      <c r="AI53" s="158"/>
-      <c r="AJ53" s="158"/>
-      <c r="AK53" s="158"/>
-      <c r="AL53" s="158"/>
-      <c r="AM53" s="158"/>
-      <c r="AN53" s="158"/>
-      <c r="AO53" s="158"/>
-      <c r="AP53" s="158"/>
-      <c r="AQ53" s="158"/>
-      <c r="AR53" s="158"/>
-      <c r="AS53" s="158"/>
-      <c r="AT53" s="158"/>
-      <c r="AU53" s="158"/>
-      <c r="AV53" s="158"/>
-      <c r="AW53" s="158"/>
-      <c r="AX53" s="158"/>
-      <c r="AY53" s="158"/>
-      <c r="AZ53" s="158"/>
-      <c r="BA53" s="158"/>
-      <c r="BB53" s="158"/>
-      <c r="BC53" s="158"/>
-      <c r="BD53" s="158"/>
-      <c r="BE53" s="158"/>
-      <c r="BF53" s="158"/>
-      <c r="BG53" s="158"/>
-      <c r="BH53" s="158"/>
-      <c r="BI53" s="158"/>
-      <c r="BJ53" s="158"/>
-      <c r="BK53" s="158"/>
-      <c r="BL53" s="158"/>
-      <c r="BM53" s="158"/>
-      <c r="BN53" s="158"/>
-      <c r="BO53" s="158"/>
-      <c r="BP53" s="159"/>
+      <c r="C53" s="159"/>
+      <c r="D53" s="159"/>
+      <c r="E53" s="159"/>
+      <c r="F53" s="159"/>
+      <c r="G53" s="159"/>
+      <c r="H53" s="159"/>
+      <c r="I53" s="159"/>
+      <c r="J53" s="159"/>
+      <c r="K53" s="159"/>
+      <c r="L53" s="159"/>
+      <c r="M53" s="159"/>
+      <c r="N53" s="159"/>
+      <c r="O53" s="159"/>
+      <c r="P53" s="159"/>
+      <c r="Q53" s="159"/>
+      <c r="R53" s="159"/>
+      <c r="S53" s="159"/>
+      <c r="T53" s="159"/>
+      <c r="U53" s="159"/>
+      <c r="V53" s="159"/>
+      <c r="W53" s="159"/>
+      <c r="X53" s="159"/>
+      <c r="Y53" s="159"/>
+      <c r="Z53" s="159"/>
+      <c r="AA53" s="159"/>
+      <c r="AB53" s="159"/>
+      <c r="AC53" s="159"/>
+      <c r="AD53" s="159"/>
+      <c r="AE53" s="159"/>
+      <c r="AF53" s="159"/>
+      <c r="AG53" s="159"/>
+      <c r="AH53" s="159"/>
+      <c r="AI53" s="159"/>
+      <c r="AJ53" s="159"/>
+      <c r="AK53" s="159"/>
+      <c r="AL53" s="159"/>
+      <c r="AM53" s="159"/>
+      <c r="AN53" s="159"/>
+      <c r="AO53" s="159"/>
+      <c r="AP53" s="159"/>
+      <c r="AQ53" s="159"/>
+      <c r="AR53" s="159"/>
+      <c r="AS53" s="159"/>
+      <c r="AT53" s="159"/>
+      <c r="AU53" s="159"/>
+      <c r="AV53" s="159"/>
+      <c r="AW53" s="159"/>
+      <c r="AX53" s="159"/>
+      <c r="AY53" s="159"/>
+      <c r="AZ53" s="159"/>
+      <c r="BA53" s="159"/>
+      <c r="BB53" s="159"/>
+      <c r="BC53" s="159"/>
+      <c r="BD53" s="159"/>
+      <c r="BE53" s="159"/>
+      <c r="BF53" s="159"/>
+      <c r="BG53" s="159"/>
+      <c r="BH53" s="159"/>
+      <c r="BI53" s="159"/>
+      <c r="BJ53" s="159"/>
+      <c r="BK53" s="159"/>
+      <c r="BL53" s="159"/>
+      <c r="BM53" s="159"/>
+      <c r="BN53" s="159"/>
+      <c r="BO53" s="159"/>
+      <c r="BP53" s="160"/>
       <c r="BQ53" s="37"/>
       <c r="BR53" s="37"/>
       <c r="BS53" s="37"/>
@@ -6038,75 +6082,75 @@
       <c r="BP66" s="62"/>
     </row>
     <row r="67" spans="1:73" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="157" t="s">
+      <c r="B67" s="158" t="s">
         <v>103</v>
       </c>
-      <c r="C67" s="158"/>
-      <c r="D67" s="158"/>
-      <c r="E67" s="158"/>
-      <c r="F67" s="158"/>
-      <c r="G67" s="158"/>
-      <c r="H67" s="158"/>
-      <c r="I67" s="158"/>
-      <c r="J67" s="158"/>
-      <c r="K67" s="158"/>
-      <c r="L67" s="158"/>
-      <c r="M67" s="158"/>
-      <c r="N67" s="158"/>
-      <c r="O67" s="158"/>
-      <c r="P67" s="158"/>
-      <c r="Q67" s="158"/>
-      <c r="R67" s="158"/>
-      <c r="S67" s="158"/>
-      <c r="T67" s="158"/>
-      <c r="U67" s="158"/>
-      <c r="V67" s="158"/>
-      <c r="W67" s="158"/>
-      <c r="X67" s="158"/>
-      <c r="Y67" s="158"/>
-      <c r="Z67" s="158"/>
-      <c r="AA67" s="158"/>
-      <c r="AB67" s="158"/>
-      <c r="AC67" s="158"/>
-      <c r="AD67" s="158"/>
-      <c r="AE67" s="158"/>
-      <c r="AF67" s="158"/>
-      <c r="AG67" s="158"/>
-      <c r="AH67" s="158"/>
-      <c r="AI67" s="158"/>
-      <c r="AJ67" s="158"/>
-      <c r="AK67" s="158"/>
-      <c r="AL67" s="158"/>
-      <c r="AM67" s="158"/>
-      <c r="AN67" s="158"/>
-      <c r="AO67" s="158"/>
-      <c r="AP67" s="158"/>
-      <c r="AQ67" s="158"/>
-      <c r="AR67" s="158"/>
-      <c r="AS67" s="158"/>
-      <c r="AT67" s="158"/>
-      <c r="AU67" s="158"/>
-      <c r="AV67" s="158"/>
-      <c r="AW67" s="158"/>
-      <c r="AX67" s="158"/>
-      <c r="AY67" s="158"/>
-      <c r="AZ67" s="158"/>
-      <c r="BA67" s="158"/>
-      <c r="BB67" s="158"/>
-      <c r="BC67" s="158"/>
-      <c r="BD67" s="158"/>
-      <c r="BE67" s="158"/>
-      <c r="BF67" s="158"/>
-      <c r="BG67" s="158"/>
-      <c r="BH67" s="158"/>
-      <c r="BI67" s="158"/>
-      <c r="BJ67" s="158"/>
-      <c r="BK67" s="158"/>
-      <c r="BL67" s="158"/>
-      <c r="BM67" s="158"/>
-      <c r="BN67" s="158"/>
-      <c r="BO67" s="158"/>
-      <c r="BP67" s="159"/>
+      <c r="C67" s="159"/>
+      <c r="D67" s="159"/>
+      <c r="E67" s="159"/>
+      <c r="F67" s="159"/>
+      <c r="G67" s="159"/>
+      <c r="H67" s="159"/>
+      <c r="I67" s="159"/>
+      <c r="J67" s="159"/>
+      <c r="K67" s="159"/>
+      <c r="L67" s="159"/>
+      <c r="M67" s="159"/>
+      <c r="N67" s="159"/>
+      <c r="O67" s="159"/>
+      <c r="P67" s="159"/>
+      <c r="Q67" s="159"/>
+      <c r="R67" s="159"/>
+      <c r="S67" s="159"/>
+      <c r="T67" s="159"/>
+      <c r="U67" s="159"/>
+      <c r="V67" s="159"/>
+      <c r="W67" s="159"/>
+      <c r="X67" s="159"/>
+      <c r="Y67" s="159"/>
+      <c r="Z67" s="159"/>
+      <c r="AA67" s="159"/>
+      <c r="AB67" s="159"/>
+      <c r="AC67" s="159"/>
+      <c r="AD67" s="159"/>
+      <c r="AE67" s="159"/>
+      <c r="AF67" s="159"/>
+      <c r="AG67" s="159"/>
+      <c r="AH67" s="159"/>
+      <c r="AI67" s="159"/>
+      <c r="AJ67" s="159"/>
+      <c r="AK67" s="159"/>
+      <c r="AL67" s="159"/>
+      <c r="AM67" s="159"/>
+      <c r="AN67" s="159"/>
+      <c r="AO67" s="159"/>
+      <c r="AP67" s="159"/>
+      <c r="AQ67" s="159"/>
+      <c r="AR67" s="159"/>
+      <c r="AS67" s="159"/>
+      <c r="AT67" s="159"/>
+      <c r="AU67" s="159"/>
+      <c r="AV67" s="159"/>
+      <c r="AW67" s="159"/>
+      <c r="AX67" s="159"/>
+      <c r="AY67" s="159"/>
+      <c r="AZ67" s="159"/>
+      <c r="BA67" s="159"/>
+      <c r="BB67" s="159"/>
+      <c r="BC67" s="159"/>
+      <c r="BD67" s="159"/>
+      <c r="BE67" s="159"/>
+      <c r="BF67" s="159"/>
+      <c r="BG67" s="159"/>
+      <c r="BH67" s="159"/>
+      <c r="BI67" s="159"/>
+      <c r="BJ67" s="159"/>
+      <c r="BK67" s="159"/>
+      <c r="BL67" s="159"/>
+      <c r="BM67" s="159"/>
+      <c r="BN67" s="159"/>
+      <c r="BO67" s="159"/>
+      <c r="BP67" s="160"/>
       <c r="BQ67" s="37"/>
       <c r="BR67" s="37"/>
       <c r="BS67" s="37"/>
@@ -6184,75 +6228,75 @@
       <c r="BQ68" s="37"/>
     </row>
     <row r="69" spans="1:73" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="157" t="s">
+      <c r="B69" s="158" t="s">
         <v>84</v>
       </c>
-      <c r="C69" s="158"/>
-      <c r="D69" s="158"/>
-      <c r="E69" s="158"/>
-      <c r="F69" s="158"/>
-      <c r="G69" s="158"/>
-      <c r="H69" s="158"/>
-      <c r="I69" s="158"/>
-      <c r="J69" s="158"/>
-      <c r="K69" s="158"/>
-      <c r="L69" s="158"/>
-      <c r="M69" s="158"/>
-      <c r="N69" s="158"/>
-      <c r="O69" s="158"/>
-      <c r="P69" s="158"/>
-      <c r="Q69" s="158"/>
-      <c r="R69" s="158"/>
-      <c r="S69" s="158"/>
-      <c r="T69" s="158"/>
-      <c r="U69" s="158"/>
-      <c r="V69" s="158"/>
-      <c r="W69" s="158"/>
-      <c r="X69" s="158"/>
-      <c r="Y69" s="158"/>
-      <c r="Z69" s="158"/>
-      <c r="AA69" s="158"/>
-      <c r="AB69" s="158"/>
-      <c r="AC69" s="158"/>
-      <c r="AD69" s="158"/>
-      <c r="AE69" s="158"/>
-      <c r="AF69" s="158"/>
-      <c r="AG69" s="158"/>
-      <c r="AH69" s="158"/>
-      <c r="AI69" s="158"/>
-      <c r="AJ69" s="158"/>
-      <c r="AK69" s="158"/>
-      <c r="AL69" s="158"/>
-      <c r="AM69" s="158"/>
-      <c r="AN69" s="158"/>
-      <c r="AO69" s="158"/>
-      <c r="AP69" s="158"/>
-      <c r="AQ69" s="158"/>
-      <c r="AR69" s="158"/>
-      <c r="AS69" s="158"/>
-      <c r="AT69" s="158"/>
-      <c r="AU69" s="158"/>
-      <c r="AV69" s="158"/>
-      <c r="AW69" s="158"/>
-      <c r="AX69" s="158"/>
-      <c r="AY69" s="158"/>
-      <c r="AZ69" s="158"/>
-      <c r="BA69" s="158"/>
-      <c r="BB69" s="158"/>
-      <c r="BC69" s="158"/>
-      <c r="BD69" s="158"/>
-      <c r="BE69" s="158"/>
-      <c r="BF69" s="158"/>
-      <c r="BG69" s="158"/>
-      <c r="BH69" s="158"/>
-      <c r="BI69" s="158"/>
-      <c r="BJ69" s="158"/>
-      <c r="BK69" s="158"/>
-      <c r="BL69" s="158"/>
-      <c r="BM69" s="158"/>
-      <c r="BN69" s="158"/>
-      <c r="BO69" s="158"/>
-      <c r="BP69" s="159"/>
+      <c r="C69" s="159"/>
+      <c r="D69" s="159"/>
+      <c r="E69" s="159"/>
+      <c r="F69" s="159"/>
+      <c r="G69" s="159"/>
+      <c r="H69" s="159"/>
+      <c r="I69" s="159"/>
+      <c r="J69" s="159"/>
+      <c r="K69" s="159"/>
+      <c r="L69" s="159"/>
+      <c r="M69" s="159"/>
+      <c r="N69" s="159"/>
+      <c r="O69" s="159"/>
+      <c r="P69" s="159"/>
+      <c r="Q69" s="159"/>
+      <c r="R69" s="159"/>
+      <c r="S69" s="159"/>
+      <c r="T69" s="159"/>
+      <c r="U69" s="159"/>
+      <c r="V69" s="159"/>
+      <c r="W69" s="159"/>
+      <c r="X69" s="159"/>
+      <c r="Y69" s="159"/>
+      <c r="Z69" s="159"/>
+      <c r="AA69" s="159"/>
+      <c r="AB69" s="159"/>
+      <c r="AC69" s="159"/>
+      <c r="AD69" s="159"/>
+      <c r="AE69" s="159"/>
+      <c r="AF69" s="159"/>
+      <c r="AG69" s="159"/>
+      <c r="AH69" s="159"/>
+      <c r="AI69" s="159"/>
+      <c r="AJ69" s="159"/>
+      <c r="AK69" s="159"/>
+      <c r="AL69" s="159"/>
+      <c r="AM69" s="159"/>
+      <c r="AN69" s="159"/>
+      <c r="AO69" s="159"/>
+      <c r="AP69" s="159"/>
+      <c r="AQ69" s="159"/>
+      <c r="AR69" s="159"/>
+      <c r="AS69" s="159"/>
+      <c r="AT69" s="159"/>
+      <c r="AU69" s="159"/>
+      <c r="AV69" s="159"/>
+      <c r="AW69" s="159"/>
+      <c r="AX69" s="159"/>
+      <c r="AY69" s="159"/>
+      <c r="AZ69" s="159"/>
+      <c r="BA69" s="159"/>
+      <c r="BB69" s="159"/>
+      <c r="BC69" s="159"/>
+      <c r="BD69" s="159"/>
+      <c r="BE69" s="159"/>
+      <c r="BF69" s="159"/>
+      <c r="BG69" s="159"/>
+      <c r="BH69" s="159"/>
+      <c r="BI69" s="159"/>
+      <c r="BJ69" s="159"/>
+      <c r="BK69" s="159"/>
+      <c r="BL69" s="159"/>
+      <c r="BM69" s="159"/>
+      <c r="BN69" s="159"/>
+      <c r="BO69" s="159"/>
+      <c r="BP69" s="160"/>
       <c r="BQ69" s="37"/>
       <c r="BR69" s="37"/>
       <c r="BS69" s="37"/>
@@ -6395,13 +6439,13 @@
       <c r="BH71" s="5"/>
       <c r="BI71" s="82"/>
       <c r="BJ71" s="5"/>
-      <c r="BK71" s="163" t="s">
+      <c r="BK71" s="164" t="s">
         <v>86</v>
       </c>
-      <c r="BL71" s="163"/>
-      <c r="BM71" s="163"/>
-      <c r="BN71" s="163"/>
-      <c r="BO71" s="163"/>
+      <c r="BL71" s="164"/>
+      <c r="BM71" s="164"/>
+      <c r="BN71" s="164"/>
+      <c r="BO71" s="164"/>
       <c r="BP71" s="12"/>
       <c r="BQ71" s="37"/>
       <c r="BR71" s="37"/>
@@ -6643,7 +6687,7 @@
       <c r="BO74" s="56"/>
       <c r="BP74" s="12"/>
       <c r="BQ74" s="37"/>
-      <c r="BR74" s="164"/>
+      <c r="BR74" s="140"/>
       <c r="BS74" s="37"/>
       <c r="BT74" s="37"/>
       <c r="BU74" s="37"/>
@@ -8850,75 +8894,75 @@
       <c r="BU103" s="37"/>
     </row>
     <row r="104" spans="2:73" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B104" s="160" t="s">
+      <c r="B104" s="161" t="s">
         <v>85</v>
       </c>
-      <c r="C104" s="161"/>
-      <c r="D104" s="161"/>
-      <c r="E104" s="161"/>
-      <c r="F104" s="161"/>
-      <c r="G104" s="161"/>
-      <c r="H104" s="161"/>
-      <c r="I104" s="161"/>
-      <c r="J104" s="161"/>
-      <c r="K104" s="161"/>
-      <c r="L104" s="161"/>
-      <c r="M104" s="161"/>
-      <c r="N104" s="161"/>
-      <c r="O104" s="161"/>
-      <c r="P104" s="161"/>
-      <c r="Q104" s="161"/>
-      <c r="R104" s="161"/>
-      <c r="S104" s="161"/>
-      <c r="T104" s="161"/>
-      <c r="U104" s="161"/>
-      <c r="V104" s="161"/>
-      <c r="W104" s="161"/>
-      <c r="X104" s="161"/>
-      <c r="Y104" s="161"/>
-      <c r="Z104" s="161"/>
-      <c r="AA104" s="161"/>
-      <c r="AB104" s="161"/>
-      <c r="AC104" s="161"/>
-      <c r="AD104" s="161"/>
-      <c r="AE104" s="161"/>
-      <c r="AF104" s="161"/>
-      <c r="AG104" s="161"/>
-      <c r="AH104" s="161"/>
-      <c r="AI104" s="161"/>
-      <c r="AJ104" s="161"/>
-      <c r="AK104" s="161"/>
-      <c r="AL104" s="161"/>
-      <c r="AM104" s="161"/>
-      <c r="AN104" s="161"/>
-      <c r="AO104" s="161"/>
-      <c r="AP104" s="161"/>
-      <c r="AQ104" s="161"/>
-      <c r="AR104" s="161"/>
-      <c r="AS104" s="161"/>
-      <c r="AT104" s="161"/>
-      <c r="AU104" s="161"/>
-      <c r="AV104" s="161"/>
-      <c r="AW104" s="161"/>
-      <c r="AX104" s="161"/>
-      <c r="AY104" s="161"/>
-      <c r="AZ104" s="161"/>
-      <c r="BA104" s="161"/>
-      <c r="BB104" s="161"/>
-      <c r="BC104" s="161"/>
-      <c r="BD104" s="161"/>
-      <c r="BE104" s="161"/>
-      <c r="BF104" s="161"/>
-      <c r="BG104" s="161"/>
-      <c r="BH104" s="161"/>
-      <c r="BI104" s="161"/>
-      <c r="BJ104" s="161"/>
-      <c r="BK104" s="161"/>
-      <c r="BL104" s="161"/>
-      <c r="BM104" s="161"/>
-      <c r="BN104" s="161"/>
-      <c r="BO104" s="161"/>
-      <c r="BP104" s="162"/>
+      <c r="C104" s="162"/>
+      <c r="D104" s="162"/>
+      <c r="E104" s="162"/>
+      <c r="F104" s="162"/>
+      <c r="G104" s="162"/>
+      <c r="H104" s="162"/>
+      <c r="I104" s="162"/>
+      <c r="J104" s="162"/>
+      <c r="K104" s="162"/>
+      <c r="L104" s="162"/>
+      <c r="M104" s="162"/>
+      <c r="N104" s="162"/>
+      <c r="O104" s="162"/>
+      <c r="P104" s="162"/>
+      <c r="Q104" s="162"/>
+      <c r="R104" s="162"/>
+      <c r="S104" s="162"/>
+      <c r="T104" s="162"/>
+      <c r="U104" s="162"/>
+      <c r="V104" s="162"/>
+      <c r="W104" s="162"/>
+      <c r="X104" s="162"/>
+      <c r="Y104" s="162"/>
+      <c r="Z104" s="162"/>
+      <c r="AA104" s="162"/>
+      <c r="AB104" s="162"/>
+      <c r="AC104" s="162"/>
+      <c r="AD104" s="162"/>
+      <c r="AE104" s="162"/>
+      <c r="AF104" s="162"/>
+      <c r="AG104" s="162"/>
+      <c r="AH104" s="162"/>
+      <c r="AI104" s="162"/>
+      <c r="AJ104" s="162"/>
+      <c r="AK104" s="162"/>
+      <c r="AL104" s="162"/>
+      <c r="AM104" s="162"/>
+      <c r="AN104" s="162"/>
+      <c r="AO104" s="162"/>
+      <c r="AP104" s="162"/>
+      <c r="AQ104" s="162"/>
+      <c r="AR104" s="162"/>
+      <c r="AS104" s="162"/>
+      <c r="AT104" s="162"/>
+      <c r="AU104" s="162"/>
+      <c r="AV104" s="162"/>
+      <c r="AW104" s="162"/>
+      <c r="AX104" s="162"/>
+      <c r="AY104" s="162"/>
+      <c r="AZ104" s="162"/>
+      <c r="BA104" s="162"/>
+      <c r="BB104" s="162"/>
+      <c r="BC104" s="162"/>
+      <c r="BD104" s="162"/>
+      <c r="BE104" s="162"/>
+      <c r="BF104" s="162"/>
+      <c r="BG104" s="162"/>
+      <c r="BH104" s="162"/>
+      <c r="BI104" s="162"/>
+      <c r="BJ104" s="162"/>
+      <c r="BK104" s="162"/>
+      <c r="BL104" s="162"/>
+      <c r="BM104" s="162"/>
+      <c r="BN104" s="162"/>
+      <c r="BO104" s="162"/>
+      <c r="BP104" s="163"/>
       <c r="BQ104" s="37"/>
       <c r="BR104" s="37"/>
       <c r="BS104" s="37"/>
@@ -11483,75 +11527,75 @@
       <c r="BP141" s="32"/>
     </row>
     <row r="142" spans="2:68" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B142" s="153" t="s">
+      <c r="B142" s="154" t="s">
         <v>77</v>
       </c>
-      <c r="C142" s="154"/>
-      <c r="D142" s="154"/>
-      <c r="E142" s="154"/>
-      <c r="F142" s="154"/>
-      <c r="G142" s="154"/>
-      <c r="H142" s="154"/>
-      <c r="I142" s="154"/>
-      <c r="J142" s="154"/>
-      <c r="K142" s="154"/>
-      <c r="L142" s="154"/>
-      <c r="M142" s="154"/>
-      <c r="N142" s="154"/>
-      <c r="O142" s="154"/>
-      <c r="P142" s="154"/>
-      <c r="Q142" s="154"/>
-      <c r="R142" s="154"/>
-      <c r="S142" s="154"/>
-      <c r="T142" s="154"/>
-      <c r="U142" s="154"/>
-      <c r="V142" s="154"/>
-      <c r="W142" s="154"/>
-      <c r="X142" s="154"/>
-      <c r="Y142" s="154"/>
-      <c r="Z142" s="154"/>
-      <c r="AA142" s="154"/>
-      <c r="AB142" s="154"/>
-      <c r="AC142" s="154"/>
-      <c r="AD142" s="154"/>
-      <c r="AE142" s="154"/>
-      <c r="AF142" s="154"/>
-      <c r="AG142" s="154"/>
-      <c r="AH142" s="154"/>
-      <c r="AI142" s="154"/>
-      <c r="AJ142" s="154"/>
-      <c r="AK142" s="154"/>
-      <c r="AL142" s="154"/>
-      <c r="AM142" s="154"/>
-      <c r="AN142" s="154"/>
-      <c r="AO142" s="154"/>
-      <c r="AP142" s="154"/>
-      <c r="AQ142" s="154"/>
-      <c r="AR142" s="154"/>
-      <c r="AS142" s="154"/>
-      <c r="AT142" s="154"/>
-      <c r="AU142" s="154"/>
-      <c r="AV142" s="154"/>
-      <c r="AW142" s="154"/>
-      <c r="AX142" s="154"/>
-      <c r="AY142" s="154"/>
-      <c r="AZ142" s="154"/>
-      <c r="BA142" s="154"/>
-      <c r="BB142" s="154"/>
-      <c r="BC142" s="154"/>
-      <c r="BD142" s="154"/>
-      <c r="BE142" s="154"/>
-      <c r="BF142" s="154"/>
-      <c r="BG142" s="154"/>
-      <c r="BH142" s="154"/>
-      <c r="BI142" s="154"/>
-      <c r="BJ142" s="154"/>
-      <c r="BK142" s="154"/>
-      <c r="BL142" s="154"/>
-      <c r="BM142" s="154"/>
-      <c r="BN142" s="154"/>
-      <c r="BO142" s="154"/>
-      <c r="BP142" s="155"/>
+      <c r="C142" s="155"/>
+      <c r="D142" s="155"/>
+      <c r="E142" s="155"/>
+      <c r="F142" s="155"/>
+      <c r="G142" s="155"/>
+      <c r="H142" s="155"/>
+      <c r="I142" s="155"/>
+      <c r="J142" s="155"/>
+      <c r="K142" s="155"/>
+      <c r="L142" s="155"/>
+      <c r="M142" s="155"/>
+      <c r="N142" s="155"/>
+      <c r="O142" s="155"/>
+      <c r="P142" s="155"/>
+      <c r="Q142" s="155"/>
+      <c r="R142" s="155"/>
+      <c r="S142" s="155"/>
+      <c r="T142" s="155"/>
+      <c r="U142" s="155"/>
+      <c r="V142" s="155"/>
+      <c r="W142" s="155"/>
+      <c r="X142" s="155"/>
+      <c r="Y142" s="155"/>
+      <c r="Z142" s="155"/>
+      <c r="AA142" s="155"/>
+      <c r="AB142" s="155"/>
+      <c r="AC142" s="155"/>
+      <c r="AD142" s="155"/>
+      <c r="AE142" s="155"/>
+      <c r="AF142" s="155"/>
+      <c r="AG142" s="155"/>
+      <c r="AH142" s="155"/>
+      <c r="AI142" s="155"/>
+      <c r="AJ142" s="155"/>
+      <c r="AK142" s="155"/>
+      <c r="AL142" s="155"/>
+      <c r="AM142" s="155"/>
+      <c r="AN142" s="155"/>
+      <c r="AO142" s="155"/>
+      <c r="AP142" s="155"/>
+      <c r="AQ142" s="155"/>
+      <c r="AR142" s="155"/>
+      <c r="AS142" s="155"/>
+      <c r="AT142" s="155"/>
+      <c r="AU142" s="155"/>
+      <c r="AV142" s="155"/>
+      <c r="AW142" s="155"/>
+      <c r="AX142" s="155"/>
+      <c r="AY142" s="155"/>
+      <c r="AZ142" s="155"/>
+      <c r="BA142" s="155"/>
+      <c r="BB142" s="155"/>
+      <c r="BC142" s="155"/>
+      <c r="BD142" s="155"/>
+      <c r="BE142" s="155"/>
+      <c r="BF142" s="155"/>
+      <c r="BG142" s="155"/>
+      <c r="BH142" s="155"/>
+      <c r="BI142" s="155"/>
+      <c r="BJ142" s="155"/>
+      <c r="BK142" s="155"/>
+      <c r="BL142" s="155"/>
+      <c r="BM142" s="155"/>
+      <c r="BN142" s="155"/>
+      <c r="BO142" s="155"/>
+      <c r="BP142" s="156"/>
     </row>
     <row r="143" spans="2:68" ht="6.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B143" s="1"/>

</xml_diff>